<commit_message>
cash drop data added
</commit_message>
<xml_diff>
--- a/CashDrop.xlsx
+++ b/CashDrop.xlsx
@@ -310,12 +310,12 @@
     <t>18010120281</t>
   </si>
   <si>
+    <t>18030103864</t>
+  </si>
+  <si>
     <t>90000023621</t>
   </si>
   <si>
-    <t>18030103864</t>
-  </si>
-  <si>
     <t>90000019687</t>
   </si>
   <si>
@@ -958,12 +958,12 @@
     <t xml:space="preserve">Madhabdi Bazar Narshingdi                                   </t>
   </si>
   <si>
+    <t xml:space="preserve">Chawmohoni Bazzar Kuliarchar                                </t>
+  </si>
+  <si>
     <t xml:space="preserve">Laxmipur Bazar Kuliarchar                                   </t>
   </si>
   <si>
-    <t xml:space="preserve">Chawmohoni Bazzar Kuliarchar                                </t>
-  </si>
-  <si>
     <t xml:space="preserve">Nurullapur Bazar Madhobdi                                   </t>
   </si>
   <si>
@@ -1378,10 +1378,10 @@
     <t xml:space="preserve">SKINV180-398827     </t>
   </si>
   <si>
+    <t xml:space="preserve">SKINV180-398805     </t>
+  </si>
+  <si>
     <t xml:space="preserve">SKINV180-398855     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV180-398805     </t>
   </si>
   <si>
     <t xml:space="preserve">SKINV180-398648     </t>
@@ -4494,7 +4494,7 @@
         <v>98</v>
       </c>
       <c r="C92" t="s">
-        <v>165</v>
+        <v>209</v>
       </c>
       <c r="D92" t="s">
         <v>314</v>
@@ -4523,7 +4523,7 @@
         <v>99</v>
       </c>
       <c r="C93" t="s">
-        <v>209</v>
+        <v>165</v>
       </c>
       <c r="D93" t="s">
         <v>315</v>

</xml_diff>